<commit_message>
Updated Accessibility Chart to help reflect Kinvey Database for Employees
</commit_message>
<xml_diff>
--- a/BCS App/Info/Accessibility Chart.xlsx
+++ b/BCS App/Info/Accessibility Chart.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="80">
   <si>
     <t>APP</t>
   </si>
@@ -252,7 +252,13 @@
     <t>Total Week OT</t>
   </si>
   <si>
-    <t>Level</t>
+    <t>Employed</t>
+  </si>
+  <si>
+    <t>Initials</t>
+  </si>
+  <si>
+    <t>Access</t>
   </si>
 </sst>
 </file>
@@ -1635,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV91"/>
+  <dimension ref="A1:IV93"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1725,7 @@
     </row>
     <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="7">
@@ -1878,9 +1884,9 @@
       <c r="L10" s="10"/>
     </row>
     <row r="11" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12" t="s">
-        <v>19</v>
+      <c r="A11" s="12"/>
+      <c r="B11" s="11" t="s">
+        <v>77</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>14</v>
@@ -1916,7 +1922,7 @@
     <row r="12" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>14</v>
@@ -1952,7 +1958,7 @@
     <row r="13" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>14</v>
@@ -1988,7 +1994,7 @@
     <row r="14" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="12" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>14</v>
@@ -2024,7 +2030,7 @@
     <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>14</v>
@@ -2060,7 +2066,7 @@
     <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>14</v>
@@ -2096,7 +2102,7 @@
     <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>14</v>
@@ -2132,7 +2138,7 @@
     <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="12" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>14</v>
@@ -2166,83 +2172,65 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L19" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
+        <v>26</v>
+      </c>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11"/>
-      <c r="B21" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H21" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="A21" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
       <c r="J21" s="10"/>
-      <c r="K21" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="K21" s="10"/>
       <c r="L21" s="10"/>
     </row>
     <row r="22" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>14</v>
@@ -2259,22 +2247,16 @@
       <c r="G22" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
       <c r="J22" s="10"/>
-      <c r="K22" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="K22" s="10"/>
       <c r="L22" s="10"/>
     </row>
     <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>14</v>
@@ -2306,7 +2288,7 @@
     <row r="24" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>14</v>
@@ -2338,7 +2320,7 @@
     <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11"/>
       <c r="B25" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>14</v>
@@ -2370,7 +2352,7 @@
     <row r="26" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="12" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>14</v>
@@ -2402,7 +2384,7 @@
     <row r="27" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>14</v>
@@ -2434,7 +2416,7 @@
     <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="12" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>14</v>
@@ -2466,7 +2448,7 @@
     <row r="29" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>14</v>
@@ -2498,7 +2480,7 @@
     <row r="30" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>14</v>
@@ -2530,7 +2512,7 @@
     <row r="31" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>14</v>
@@ -2562,7 +2544,7 @@
     <row r="32" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11"/>
       <c r="B32" s="12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>14</v>
@@ -2594,7 +2576,7 @@
     <row r="33" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>14</v>
@@ -2626,7 +2608,7 @@
     <row r="34" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>14</v>
@@ -2658,7 +2640,7 @@
     <row r="35" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>14</v>
@@ -2722,7 +2704,7 @@
     <row r="37" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>14</v>
@@ -2754,7 +2736,7 @@
     <row r="38" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>14</v>
@@ -2786,7 +2768,7 @@
     <row r="39" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>14</v>
@@ -2818,7 +2800,7 @@
     <row r="40" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>14</v>
@@ -2850,7 +2832,7 @@
     <row r="41" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11"/>
       <c r="B41" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>14</v>
@@ -2880,25 +2862,41 @@
       <c r="L41" s="10"/>
     </row>
     <row r="42" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
-      <c r="G42" s="10"/>
-      <c r="H42" s="10"/>
-      <c r="I42" s="10"/>
+      <c r="A42" s="11"/>
+      <c r="B42" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J42" s="10"/>
-      <c r="K42" s="10"/>
+      <c r="K42" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="L42" s="10"/>
     </row>
     <row r="43" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>14</v>
@@ -2915,50 +2913,38 @@
       <c r="G43" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H43" s="10"/>
-      <c r="I43" s="10"/>
+      <c r="H43" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J43" s="10"/>
-      <c r="K43" s="10"/>
+      <c r="K43" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="L43" s="10"/>
     </row>
     <row r="44" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="11"/>
-      <c r="B44" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E44" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F44" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H44" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I44" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="A44" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="10"/>
       <c r="J44" s="10"/>
-      <c r="K44" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L44" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="K44" s="10"/>
+      <c r="L44" s="10"/>
     </row>
     <row r="45" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="12" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>14</v>
@@ -2975,24 +2961,16 @@
       <c r="G45" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H45" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I45" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="H45" s="10"/>
+      <c r="I45" s="10"/>
       <c r="J45" s="10"/>
-      <c r="K45" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L45" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
     </row>
     <row r="46" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>14</v>
@@ -3026,7 +3004,7 @@
     <row r="47" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>14</v>
@@ -3060,7 +3038,7 @@
     <row r="48" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>14</v>
@@ -3094,7 +3072,7 @@
     <row r="49" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="12" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>14</v>
@@ -3128,7 +3106,7 @@
     <row r="50" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11"/>
       <c r="B50" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>14</v>
@@ -3162,7 +3140,7 @@
     <row r="51" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>14</v>
@@ -3196,7 +3174,7 @@
     <row r="52" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="12" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>14</v>
@@ -3230,7 +3208,7 @@
     <row r="53" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>14</v>
@@ -3264,7 +3242,7 @@
     <row r="54" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="12" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>14</v>
@@ -3298,7 +3276,7 @@
     <row r="55" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="B55" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>14</v>
@@ -3330,25 +3308,43 @@
       </c>
     </row>
     <row r="56" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B56" s="11"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
-      <c r="G56" s="10"/>
-      <c r="H56" s="10"/>
-      <c r="I56" s="10"/>
+      <c r="A56" s="11"/>
+      <c r="B56" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E56" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J56" s="10"/>
-      <c r="K56" s="10"/>
-      <c r="L56" s="10"/>
+      <c r="K56" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L56" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="57" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="B57" s="12" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>14</v>
@@ -3365,50 +3361,40 @@
       <c r="G57" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H57" s="10"/>
-      <c r="I57" s="10"/>
+      <c r="H57" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J57" s="10"/>
-      <c r="K57" s="10"/>
-      <c r="L57" s="10"/>
+      <c r="K57" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L57" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="58" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="11"/>
-      <c r="B58" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C58" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D58" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E58" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F58" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G58" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H58" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I58" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="A58" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="11"/>
+      <c r="C58" s="10"/>
+      <c r="D58" s="10"/>
+      <c r="E58" s="10"/>
+      <c r="F58" s="10"/>
+      <c r="G58" s="10"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
       <c r="J58" s="10"/>
-      <c r="K58" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L58" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="K58" s="10"/>
+      <c r="L58" s="10"/>
     </row>
     <row r="59" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="11"/>
       <c r="B59" s="12" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>14</v>
@@ -3425,24 +3411,16 @@
       <c r="G59" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H59" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I59" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="H59" s="10"/>
+      <c r="I59" s="10"/>
       <c r="J59" s="10"/>
-      <c r="K59" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L59" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="K59" s="10"/>
+      <c r="L59" s="10"/>
     </row>
     <row r="60" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="11"/>
       <c r="B60" s="12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>14</v>
@@ -3476,7 +3454,7 @@
     <row r="61" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="11"/>
       <c r="B61" s="12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>14</v>
@@ -3510,7 +3488,7 @@
     <row r="62" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
       <c r="B62" s="12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>14</v>
@@ -3544,7 +3522,7 @@
     <row r="63" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="11"/>
       <c r="B63" s="12" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>14</v>
@@ -3578,7 +3556,7 @@
     <row r="64" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>14</v>
@@ -3612,7 +3590,7 @@
     <row r="65" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="11"/>
       <c r="B65" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>14</v>
@@ -3646,7 +3624,7 @@
     <row r="66" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="11"/>
       <c r="B66" s="12" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>14</v>
@@ -3680,7 +3658,7 @@
     <row r="67" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="11"/>
       <c r="B67" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>14</v>
@@ -3714,7 +3692,7 @@
     <row r="68" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="11"/>
       <c r="B68" s="12" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C68" s="13" t="s">
         <v>14</v>
@@ -3748,7 +3726,7 @@
     <row r="69" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="11"/>
       <c r="B69" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C69" s="13" t="s">
         <v>14</v>
@@ -3780,25 +3758,43 @@
       </c>
     </row>
     <row r="70" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B70" s="11"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="10"/>
-      <c r="E70" s="10"/>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
-      <c r="H70" s="10"/>
-      <c r="I70" s="10"/>
+      <c r="A70" s="11"/>
+      <c r="B70" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D70" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E70" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I70" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J70" s="10"/>
-      <c r="K70" s="10"/>
-      <c r="L70" s="10"/>
+      <c r="K70" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L70" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="71" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C71" s="13" t="s">
         <v>14</v>
@@ -3815,52 +3811,40 @@
       <c r="G71" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H71" s="10"/>
-      <c r="I71" s="10"/>
+      <c r="H71" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I71" s="13" t="s">
+        <v>14</v>
+      </c>
       <c r="J71" s="10"/>
-      <c r="K71" s="10"/>
-      <c r="L71" s="10"/>
+      <c r="K71" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L71" s="13" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="72" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="11"/>
-      <c r="B72" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C72" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D72" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E72" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F72" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G72" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H72" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I72" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J72" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K72" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L72" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="A72" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B72" s="11"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+      <c r="H72" s="10"/>
+      <c r="I72" s="10"/>
+      <c r="J72" s="10"/>
+      <c r="K72" s="10"/>
+      <c r="L72" s="10"/>
     </row>
     <row r="73" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="11"/>
       <c r="B73" s="12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C73" s="13" t="s">
         <v>14</v>
@@ -3877,26 +3861,16 @@
       <c r="G73" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="H73" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I73" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J73" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K73" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L73" s="13" t="s">
-        <v>14</v>
-      </c>
+      <c r="H73" s="10"/>
+      <c r="I73" s="10"/>
+      <c r="J73" s="10"/>
+      <c r="K73" s="10"/>
+      <c r="L73" s="10"/>
     </row>
     <row r="74" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="11"/>
       <c r="B74" s="12" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>14</v>
@@ -3932,7 +3906,7 @@
     <row r="75" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="11"/>
       <c r="B75" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>14</v>
@@ -3968,7 +3942,7 @@
     <row r="76" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11"/>
       <c r="B76" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>14</v>
@@ -4004,7 +3978,7 @@
     <row r="77" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="11"/>
       <c r="B77" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>14</v>
@@ -4040,7 +4014,7 @@
     <row r="78" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="11"/>
       <c r="B78" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>14</v>
@@ -4076,7 +4050,7 @@
     <row r="79" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="11"/>
       <c r="B79" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C79" s="13" t="s">
         <v>14</v>
@@ -4112,7 +4086,7 @@
     <row r="80" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="11"/>
       <c r="B80" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>14</v>
@@ -4148,7 +4122,7 @@
     <row r="81" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11"/>
       <c r="B81" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>14</v>
@@ -4184,7 +4158,7 @@
     <row r="82" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="11"/>
       <c r="B82" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>14</v>
@@ -4220,7 +4194,7 @@
     <row r="83" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="11"/>
       <c r="B83" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>14</v>
@@ -4256,7 +4230,7 @@
     <row r="84" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="12" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C84" s="13" t="s">
         <v>14</v>
@@ -4292,7 +4266,7 @@
     <row r="85" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="11"/>
       <c r="B85" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>14</v>
@@ -4328,7 +4302,7 @@
     <row r="86" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="11"/>
       <c r="B86" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C86" s="13" t="s">
         <v>14</v>
@@ -4364,7 +4338,7 @@
     <row r="87" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="11"/>
       <c r="B87" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C87" s="13" t="s">
         <v>14</v>
@@ -4400,7 +4374,7 @@
     <row r="88" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="11"/>
       <c r="B88" s="12" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C88" s="13" t="s">
         <v>14</v>
@@ -4436,7 +4410,7 @@
     <row r="89" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="11"/>
       <c r="B89" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C89" s="13" t="s">
         <v>14</v>
@@ -4472,7 +4446,7 @@
     <row r="90" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="11"/>
       <c r="B90" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C90" s="13" t="s">
         <v>14</v>
@@ -4508,36 +4482,108 @@
     <row r="91" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="11"/>
       <c r="B91" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C91" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D91" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F91" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G91" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I91" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J91" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K91" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L91" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="11"/>
+      <c r="B92" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="C92" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D92" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E92" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F92" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G92" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H92" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I92" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J92" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K92" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L92" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="11"/>
+      <c r="B93" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C91" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D91" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E91" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F91" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="G91" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H91" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I91" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="J91" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="K91" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L91" s="13" t="s">
+      <c r="C93" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D93" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E93" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F93" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H93" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I93" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J93" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K93" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="L93" s="13" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>